<commit_message>
add chick is working , add cage and birds work as well
</commit_message>
<xml_diff>
--- a/ProjectBirdsz/bin/Debug/birds.xlsx
+++ b/ProjectBirdsz/bin/Debug/birds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyal\OneDrive\Desktop\FinalPROJECTbirds\ProjectBirdsz\ProjectBirdsz\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0017302D-859F-47D9-B40B-5AC758713ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72942792-83DB-437D-A850-3F03BE3EB35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22905" yWindow="3720" windowWidth="14475" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -25,25 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
-  <si>
-    <t>Guy</t>
-  </si>
-  <si>
-    <t>Aloosh</t>
-  </si>
-  <si>
-    <t>today</t>
-  </si>
-  <si>
-    <t>man</t>
-  </si>
-  <si>
-    <t>Haliva</t>
-  </si>
-  <si>
-    <t>tomorrow</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>SerialNumber</t>
   </si>
@@ -67,6 +49,24 @@
   </si>
   <si>
     <t>MotherSerialNumber</t>
+  </si>
+  <si>
+    <t>SerialBird</t>
+  </si>
+  <si>
+    <t>Sub Species</t>
+  </si>
+  <si>
+    <t>Date of Bird</t>
+  </si>
+  <si>
+    <t>Cage  Number</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Mother</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -394,106 +394,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting foam with progress bar
</commit_message>
<xml_diff>
--- a/ProjectBirdsz/bin/Debug/birds.xlsx
+++ b/ProjectBirdsz/bin/Debug/birds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyal\OneDrive\Desktop\FinalPROJECTbirds\ProjectBirdsz\ProjectBirdsz\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72942792-83DB-437D-A850-3F03BE3EB35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F84E2BC-DE32-4A36-AB75-4A10B7C9F790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22905" yWindow="3720" windowWidth="14475" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>SerialNumber</t>
   </si>
@@ -51,22 +51,13 @@
     <t>MotherSerialNumber</t>
   </si>
   <si>
-    <t>SerialBird</t>
-  </si>
-  <si>
-    <t>Sub Species</t>
-  </si>
-  <si>
-    <t>Date of Bird</t>
-  </si>
-  <si>
-    <t>Cage  Number</t>
-  </si>
-  <si>
-    <t>Father</t>
-  </si>
-  <si>
-    <t>Mother</t>
+    <t>Golden</t>
+  </si>
+  <si>
+    <t>Amrican</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
@@ -102,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -419,55 +411,29 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1">
+        <v>35490</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>100</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
-        <v>100</v>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checking name or password is valid, adding some message boxs
</commit_message>
<xml_diff>
--- a/ProjectBirdsz/bin/Debug/birds.xlsx
+++ b/ProjectBirdsz/bin/Debug/birds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="חוברת_עבודה_זו"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyal\source\repos\NewBirds\ProjectBirdsz\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyal\Source\Repos\NewBirds\ProjectBirdsz\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D1C4D4-E8DF-40CC-91EC-893A23968206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBF9A90-150D-4FA0-B21F-FC22D92679E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>SerialNumber</t>
   </si>
@@ -66,16 +66,16 @@
     <t>Golden Amrican</t>
   </si>
   <si>
-    <t>Notrh America</t>
+    <t>West Europe</t>
+  </si>
+  <si>
+    <t>Central America</t>
   </si>
   <si>
     <t xml:space="preserve">Golden Australian </t>
   </si>
   <si>
     <t>Coastal cities</t>
-  </si>
-  <si>
-    <t>West Europe</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="גיליון1"/>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
@@ -439,33 +439,33 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1">
-        <v>45054</v>
+        <v>45077</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -477,7 +477,7 @@
         <v>45077</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -486,18 +486,18 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>45077</v>
@@ -506,10 +506,10 @@
         <v>11</v>
       </c>
       <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
         <v>1</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -517,13 +517,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1">
         <v>45047</v>
@@ -532,69 +532,173 @@
         <v>11</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
-        <v>45047</v>
+        <v>45077</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1">
         <v>45077</v>
       </c>
       <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45054</v>
+      </c>
+      <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45047</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45077</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45047</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H7">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H11">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel adding birds and cages
</commit_message>
<xml_diff>
--- a/ProjectBirdsz/bin/Debug/birds.xlsx
+++ b/ProjectBirdsz/bin/Debug/birds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyal\Source\Repos\NewBirds\ProjectBirdsz\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4547280-4454-43D3-906E-537FAC08D309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A7A8AE-AF08-4C74-A2EE-2FA2F26172FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
   <si>
     <t>SerialNumber</t>
   </si>
@@ -405,7 +405,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="גיליון1"/>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
@@ -672,7 +672,7 @@
         <v>11</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>4</v>
@@ -683,84 +683,185 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1">
-        <v>45077</v>
+        <v>45047</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1">
-        <v>45047</v>
+        <v>45075</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45074</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45082</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="H14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45078</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45083</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>11</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>17</v>
       </c>
-      <c r="D13" s="1">
-        <v>45075</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <v>6</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <v>4</v>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45077</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>